<commit_message>
Update case01 in exp2
</commit_message>
<xml_diff>
--- a/exp2/case01/report/correlation-interactions/SimpleCorrPairAnalysis-strong.xlsx
+++ b/exp2/case01/report/correlation-interactions/SimpleCorrPairAnalysis-strong.xlsx
@@ -6,16 +6,16 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="strong_spearman_16" r:id="rId3" sheetId="1"/>
-    <sheet name="strong_pearson_24" r:id="rId4" sheetId="2"/>
+    <sheet name="strong_spearman_26" r:id="rId3" sheetId="1"/>
+    <sheet name="strong_spearman_43" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="45">
-  <si>
-    <t>Correlation information for DiffTheta - NroNecessaryInteractions in non-gamified.Master using the method: spearman</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="52">
+  <si>
+    <t>Correlation information for DiffScore - NroDesiredInteractions in ont-gamified.Apprentice using the method: spearman</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -24,10 +24,10 @@
     <t>Correlation matrix</t>
   </si>
   <si>
-    <t>DiffTheta</t>
-  </si>
-  <si>
-    <t>NroNecessaryInteractions</t>
+    <t>DiffScore</t>
+  </si>
+  <si>
+    <t>NroDesiredInteractions</t>
   </si>
   <si>
     <t>Matrix of t-test value</t>
@@ -51,13 +51,13 @@
     <t>p</t>
   </si>
   <si>
-    <t>DffTh-NrNcI</t>
-  </si>
-  <si>
-    <t>Data source for DiffTheta - NroNecessaryInteractions in non-gamified.Master</t>
-  </si>
-  <si>
-    <t>Data full source for DiffTheta - NroNecessaryInteractions in non-gamified.Master</t>
+    <t>DffSc-NrDsI</t>
+  </si>
+  <si>
+    <t>Data source for DiffScore - NroDesiredInteractions in ont-gamified.Apprentice</t>
+  </si>
+  <si>
+    <t>Data full source for DiffScore - NroDesiredInteractions in ont-gamified.Apprentice</t>
   </si>
   <si>
     <t>UserID</t>
@@ -78,76 +78,97 @@
     <t>PlayerRole</t>
   </si>
   <si>
+    <t>ont-gamified</t>
+  </si>
+  <si>
+    <t>Grupo Afrodite</t>
+  </si>
+  <si>
+    <t>Grupo Cronus</t>
+  </si>
+  <si>
+    <t>Grupo Hélio</t>
+  </si>
+  <si>
+    <t>Grupo Ares</t>
+  </si>
+  <si>
+    <t>Grupo Zeus</t>
+  </si>
+  <si>
+    <t>Grupo Urano</t>
+  </si>
+  <si>
+    <t>Grupo Hefesto</t>
+  </si>
+  <si>
+    <t>Grupo Gaia</t>
+  </si>
+  <si>
+    <t>Grupo Apolo</t>
+  </si>
+  <si>
+    <t>Grupo Hades</t>
+  </si>
+  <si>
+    <t>Grupo Artemis</t>
+  </si>
+  <si>
+    <t>Grupo Hermes</t>
+  </si>
+  <si>
+    <t>Grupo Caronte</t>
+  </si>
+  <si>
+    <t>Apprentice</t>
+  </si>
+  <si>
+    <t>Yee Achiever</t>
+  </si>
+  <si>
+    <t>Yee Socializer</t>
+  </si>
+  <si>
+    <t>Correlation information for DiffScore - Interest/Enjoyment in non-gamified.Master using the method: spearman</t>
+  </si>
+  <si>
+    <t>Interest/Enjoyment</t>
+  </si>
+  <si>
+    <t>DffSc-Int/E</t>
+  </si>
+  <si>
+    <t>Data source for DiffScore - Interest/Enjoyment in non-gamified.Master</t>
+  </si>
+  <si>
+    <t>Data full source for DiffScore - Interest/Enjoyment in non-gamified.Master</t>
+  </si>
+  <si>
     <t>non-gamified</t>
   </si>
   <si>
-    <t>Grupo Team 9</t>
-  </si>
-  <si>
     <t>Grupo Team 10</t>
   </si>
   <si>
+    <t>Grupo Team 3</t>
+  </si>
+  <si>
     <t>Grupo  Team 6</t>
   </si>
   <si>
-    <t>Grupo Team 4</t>
-  </si>
-  <si>
-    <t>Grupo Team 5</t>
-  </si>
-  <si>
-    <t>Grupo Team 15</t>
-  </si>
-  <si>
     <t>Grupo Team 12</t>
   </si>
   <si>
-    <t>Grupo Team 16</t>
-  </si>
-  <si>
     <t>Grupo Team 8</t>
   </si>
   <si>
     <t>Grupo Team 14</t>
   </si>
   <si>
-    <t>Grupo Team 7</t>
-  </si>
-  <si>
     <t>Master</t>
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>Correlation information for DiffTheta - NroDesiredInteractions in non-gamified.Apprentice using the method: pearson</t>
-  </si>
-  <si>
-    <t>NroDesiredInteractions</t>
-  </si>
-  <si>
-    <t>DffTh-NrDsI</t>
-  </si>
-  <si>
-    <t>Data source for DiffTheta - NroDesiredInteractions in non-gamified.Apprentice</t>
-  </si>
-  <si>
-    <t>Data full source for DiffTheta - NroDesiredInteractions in non-gamified.Apprentice</t>
-  </si>
-  <si>
-    <t>Grupo Team 11</t>
-  </si>
-  <si>
-    <t>Grupo Team 3</t>
-  </si>
-  <si>
-    <t>Grupo Team 2</t>
-  </si>
-  <si>
-    <t>Grupo Team 13</t>
-  </si>
-  <si>
-    <t>Apprentice</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1563,7 @@
         <v>1.0</v>
       </c>
       <c r="C6" t="n" s="32">
-        <v>0.7193787788820487</v>
+        <v>0.7906659377718414</v>
       </c>
     </row>
     <row r="7">
@@ -1550,7 +1571,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="n" s="31">
-        <v>0.7193787788820487</v>
+        <v>0.7906659377718414</v>
       </c>
       <c r="C7" t="n" s="32">
         <v>1.0</v>
@@ -1588,7 +1609,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C12" t="n" s="52">
-        <v>3.1069398172122877</v>
+        <v>4.283138670760518</v>
       </c>
     </row>
     <row r="13">
@@ -1596,7 +1617,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="n" s="51">
-        <v>3.1069398172122877</v>
+        <v>4.283138670760518</v>
       </c>
       <c r="C13" t="e" s="52">
         <v>#DIV/0!</v>
@@ -1634,7 +1655,7 @@
         <v>0.0</v>
       </c>
       <c r="C18" t="n" s="72">
-        <v>0.012580804297016357</v>
+        <v>0.001291911550344249</v>
       </c>
     </row>
     <row r="19">
@@ -1642,7 +1663,7 @@
         <v>4</v>
       </c>
       <c r="B19" t="n" s="71">
-        <v>0.012580804297016357</v>
+        <v>0.001291911550344249</v>
       </c>
       <c r="C19" t="n" s="72">
         <v>0.0</v>
@@ -1683,16 +1704,16 @@
         <v>12</v>
       </c>
       <c r="B24" t="n" s="91">
-        <v>0.21022272314811144</v>
+        <v>0.42469858088516815</v>
       </c>
       <c r="C24" t="n" s="92">
-        <v>0.7193787788820487</v>
+        <v>0.7906659377718414</v>
       </c>
       <c r="D24" t="n" s="93">
-        <v>0.921564350442949</v>
+        <v>0.9345283476119869</v>
       </c>
       <c r="E24" t="n" s="94">
-        <v>0.012580804297016357</v>
+        <v>0.001291911550344249</v>
       </c>
     </row>
     <row r="25">
@@ -1720,417 +1741,485 @@
     </row>
     <row r="29">
       <c r="A29" t="n" s="113">
-        <v>-0.16206083851899455</v>
+        <v>2.251388888888889</v>
       </c>
       <c r="B29" t="n" s="114">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n" s="113">
-        <v>-1.0314610011269332</v>
+        <v>1.2369047619047615</v>
       </c>
       <c r="B30" t="n" s="114">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n" s="113">
-        <v>0.728136309206279</v>
+        <v>1.6660714285714286</v>
       </c>
       <c r="B31" t="n" s="114">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n" s="113">
-        <v>-0.16226149413174898</v>
+        <v>2.4222222222222207</v>
       </c>
       <c r="B32" t="n" s="114">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n" s="113">
-        <v>0.3544640659509295</v>
+        <v>1.2958333333333343</v>
       </c>
       <c r="B33" t="n" s="114">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n" s="113">
-        <v>-0.14299820329426893</v>
+        <v>1.0882936507936503</v>
       </c>
       <c r="B34" t="n" s="114">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n" s="113">
-        <v>0.6172103617216727</v>
+        <v>3.2472222222222227</v>
       </c>
       <c r="B35" t="n" s="114">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n" s="113">
-        <v>0.4733407256476818</v>
+        <v>2.2138888888888886</v>
       </c>
       <c r="B36" t="n" s="114">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n" s="113">
-        <v>-0.548850785325394</v>
+        <v>3.0138888888888884</v>
       </c>
       <c r="B37" t="n" s="114">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n" s="113">
-        <v>0.6361517246417284</v>
+        <v>1.7291666666666679</v>
       </c>
       <c r="B38" t="n" s="114">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n" s="113">
-        <v>-0.5466262379416822</v>
+        <v>2.6500000000000004</v>
       </c>
       <c r="B39" t="n" s="114">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s">
+      <c r="A40" t="n" s="113">
+        <v>0.42777777777777715</v>
+      </c>
+      <c r="B40" t="n" s="114">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n" s="113">
+        <v>1.8666666666666671</v>
+      </c>
+      <c r="B41" t="n" s="114">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="s">
+    <row r="43">
+      <c r="A43" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="s" s="118">
+    <row r="44">
+      <c r="A44" t="s" s="118">
         <v>14</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="s" s="132">
+    <row r="45">
+      <c r="A45" t="s" s="132">
         <v>15</v>
       </c>
-      <c r="B43" t="s" s="132">
+      <c r="B45" t="s" s="132">
         <v>16</v>
       </c>
-      <c r="C43" t="s" s="132">
+      <c r="C45" t="s" s="132">
         <v>17</v>
       </c>
-      <c r="D43" t="s" s="132">
+      <c r="D45" t="s" s="132">
         <v>18</v>
       </c>
-      <c r="E43" t="s" s="132">
+      <c r="E45" t="s" s="132">
         <v>19</v>
       </c>
-      <c r="F43" t="s" s="132">
+      <c r="F45" t="s" s="132">
         <v>20</v>
       </c>
-      <c r="G43" t="s" s="132">
+      <c r="G45" t="s" s="132">
         <v>3</v>
       </c>
-      <c r="H43" t="s" s="132">
+      <c r="H45" t="s" s="132">
         <v>4</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n" s="133">
-        <v>10179.0</v>
-      </c>
-      <c r="B44" t="n" s="134">
-        <v>1.0310759E7</v>
-      </c>
-      <c r="C44" t="s" s="135">
-        <v>21</v>
-      </c>
-      <c r="D44" t="s" s="136">
-        <v>22</v>
-      </c>
-      <c r="E44" t="s" s="137">
-        <v>33</v>
-      </c>
-      <c r="F44" t="s" s="138">
-        <v>34</v>
-      </c>
-      <c r="G44" t="n" s="139">
-        <v>-0.16206083851899455</v>
-      </c>
-      <c r="H44" t="n" s="140">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n" s="133">
-        <v>10181.0</v>
-      </c>
-      <c r="B45" t="n" s="134">
-        <v>1.0276866E7</v>
-      </c>
-      <c r="C45" t="s" s="135">
-        <v>21</v>
-      </c>
-      <c r="D45" t="s" s="136">
-        <v>23</v>
-      </c>
-      <c r="E45" t="s" s="137">
-        <v>33</v>
-      </c>
-      <c r="F45" t="s" s="138">
-        <v>34</v>
-      </c>
-      <c r="G45" t="n" s="139">
-        <v>-1.0314610011269332</v>
-      </c>
-      <c r="H45" t="n" s="140">
-        <v>2.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n" s="133">
-        <v>10191.0</v>
+        <v>10170.0</v>
       </c>
       <c r="B46" t="n" s="134">
-        <v>1.0276981E7</v>
+        <v>1.0260351E7</v>
       </c>
       <c r="C46" t="s" s="135">
         <v>21</v>
       </c>
       <c r="D46" t="s" s="136">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E46" t="s" s="137">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F46" t="s" s="138">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G46" t="n" s="139">
-        <v>0.728136309206279</v>
+        <v>2.251388888888889</v>
       </c>
       <c r="H46" t="n" s="140">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n" s="133">
-        <v>10212.0</v>
+        <v>10176.0</v>
       </c>
       <c r="B47" t="n" s="134">
-        <v>9065750.0</v>
+        <v>1.0276949E7</v>
       </c>
       <c r="C47" t="s" s="135">
         <v>21</v>
       </c>
       <c r="D47" t="s" s="136">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E47" t="s" s="137">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F47" t="s" s="138">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G47" t="n" s="139">
-        <v>-0.16226149413174898</v>
+        <v>1.2369047619047615</v>
       </c>
       <c r="H47" t="n" s="140">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n" s="133">
-        <v>10214.0</v>
+        <v>10183.0</v>
       </c>
       <c r="B48" t="n" s="134">
-        <v>1.0277022E7</v>
+        <v>1.035203E7</v>
       </c>
       <c r="C48" t="s" s="135">
         <v>21</v>
       </c>
       <c r="D48" t="s" s="136">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E48" t="s" s="137">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F48" t="s" s="138">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G48" t="n" s="139">
-        <v>0.3544640659509295</v>
+        <v>1.6660714285714286</v>
       </c>
       <c r="H48" t="n" s="140">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n" s="133">
-        <v>10216.0</v>
+        <v>10186.0</v>
       </c>
       <c r="B49" t="n" s="134">
-        <v>1.027672E7</v>
+        <v>1.0310551E7</v>
       </c>
       <c r="C49" t="s" s="135">
         <v>21</v>
       </c>
       <c r="D49" t="s" s="136">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E49" t="s" s="137">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F49" t="s" s="138">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G49" t="n" s="139">
-        <v>-0.14299820329426893</v>
+        <v>2.4222222222222207</v>
       </c>
       <c r="H49" t="n" s="140">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n" s="133">
-        <v>10219.0</v>
+        <v>10190.0</v>
       </c>
       <c r="B50" t="n" s="134">
-        <v>1.0276831E7</v>
+        <v>1.0276907E7</v>
       </c>
       <c r="C50" t="s" s="135">
         <v>21</v>
       </c>
       <c r="D50" t="s" s="136">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E50" t="s" s="137">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F50" t="s" s="138">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G50" t="n" s="139">
-        <v>0.6172103617216727</v>
+        <v>1.2958333333333343</v>
       </c>
       <c r="H50" t="n" s="140">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n" s="133">
-        <v>10222.0</v>
+        <v>10195.0</v>
       </c>
       <c r="B51" t="n" s="134">
-        <v>9436110.0</v>
+        <v>1.0351971E7</v>
       </c>
       <c r="C51" t="s" s="135">
         <v>21</v>
       </c>
       <c r="D51" t="s" s="136">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E51" t="s" s="137">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F51" t="s" s="138">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G51" t="n" s="139">
-        <v>0.4733407256476818</v>
+        <v>1.0882936507936503</v>
       </c>
       <c r="H51" t="n" s="140">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n" s="133">
-        <v>10226.0</v>
+        <v>10196.0</v>
       </c>
       <c r="B52" t="n" s="134">
-        <v>1.0310342E7</v>
+        <v>1.0310655E7</v>
       </c>
       <c r="C52" t="s" s="135">
         <v>21</v>
       </c>
       <c r="D52" t="s" s="136">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E52" t="s" s="137">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F52" t="s" s="138">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G52" t="n" s="139">
-        <v>-0.548850785325394</v>
+        <v>3.2472222222222227</v>
       </c>
       <c r="H52" t="n" s="140">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n" s="133">
-        <v>10230.0</v>
+        <v>10197.0</v>
       </c>
       <c r="B53" t="n" s="134">
-        <v>1.0351992E7</v>
+        <v>1.0276661E7</v>
       </c>
       <c r="C53" t="s" s="135">
         <v>21</v>
       </c>
       <c r="D53" t="s" s="136">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E53" t="s" s="137">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F53" t="s" s="138">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G53" t="n" s="139">
-        <v>0.6361517246417284</v>
+        <v>2.2138888888888886</v>
       </c>
       <c r="H53" t="n" s="140">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n" s="133">
-        <v>10234.0</v>
+        <v>10198.0</v>
       </c>
       <c r="B54" t="n" s="134">
-        <v>1.0310676E7</v>
+        <v>1.0310888E7</v>
       </c>
       <c r="C54" t="s" s="135">
         <v>21</v>
       </c>
       <c r="D54" t="s" s="136">
+        <v>30</v>
+      </c>
+      <c r="E54" t="s" s="137">
+        <v>35</v>
+      </c>
+      <c r="F54" t="s" s="138">
+        <v>37</v>
+      </c>
+      <c r="G54" t="n" s="139">
+        <v>3.0138888888888884</v>
+      </c>
+      <c r="H54" t="n" s="140">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n" s="133">
+        <v>10200.0</v>
+      </c>
+      <c r="B55" t="n" s="134">
+        <v>9795272.0</v>
+      </c>
+      <c r="C55" t="s" s="135">
+        <v>21</v>
+      </c>
+      <c r="D55" t="s" s="136">
+        <v>31</v>
+      </c>
+      <c r="E55" t="s" s="137">
+        <v>35</v>
+      </c>
+      <c r="F55" t="s" s="138">
+        <v>37</v>
+      </c>
+      <c r="G55" t="n" s="139">
+        <v>1.7291666666666679</v>
+      </c>
+      <c r="H55" t="n" s="140">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n" s="133">
+        <v>10209.0</v>
+      </c>
+      <c r="B56" t="n" s="134">
+        <v>1.0262669E7</v>
+      </c>
+      <c r="C56" t="s" s="135">
+        <v>21</v>
+      </c>
+      <c r="D56" t="s" s="136">
         <v>32</v>
       </c>
-      <c r="E54" t="s" s="137">
+      <c r="E56" t="s" s="137">
+        <v>35</v>
+      </c>
+      <c r="F56" t="s" s="138">
+        <v>36</v>
+      </c>
+      <c r="G56" t="n" s="139">
+        <v>2.6500000000000004</v>
+      </c>
+      <c r="H56" t="n" s="140">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n" s="133">
+        <v>10221.0</v>
+      </c>
+      <c r="B57" t="n" s="134">
+        <v>9082496.0</v>
+      </c>
+      <c r="C57" t="s" s="135">
+        <v>21</v>
+      </c>
+      <c r="D57" t="s" s="136">
         <v>33</v>
       </c>
-      <c r="F54" t="s" s="138">
+      <c r="E57" t="s" s="137">
+        <v>35</v>
+      </c>
+      <c r="F57" t="s" s="138">
+        <v>36</v>
+      </c>
+      <c r="G57" t="n" s="139">
+        <v>0.42777777777777715</v>
+      </c>
+      <c r="H57" t="n" s="140">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n" s="133">
+        <v>10231.0</v>
+      </c>
+      <c r="B58" t="n" s="134">
+        <v>1.0276911E7</v>
+      </c>
+      <c r="C58" t="s" s="135">
+        <v>21</v>
+      </c>
+      <c r="D58" t="s" s="136">
         <v>34</v>
       </c>
-      <c r="G54" t="n" s="139">
-        <v>-0.5466262379416822</v>
-      </c>
-      <c r="H54" t="n" s="140">
-        <v>2.0</v>
+      <c r="E58" t="s" s="137">
+        <v>35</v>
+      </c>
+      <c r="F58" t="s" s="138">
+        <v>36</v>
+      </c>
+      <c r="G58" t="n" s="139">
+        <v>1.8666666666666671</v>
+      </c>
+      <c r="H58" t="n" s="140">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -2159,7 +2248,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="142">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
@@ -2183,7 +2272,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s" s="170">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6">
@@ -2194,18 +2283,18 @@
         <v>1.0</v>
       </c>
       <c r="C6" t="n" s="172">
-        <v>-0.7192730061032833</v>
+        <v>-0.8696565534786727</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="166">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" t="n" s="171">
-        <v>-0.7192730061032833</v>
+        <v>-0.8696565534786727</v>
       </c>
       <c r="C7" t="n" s="172">
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
     </row>
     <row r="8">
@@ -2229,7 +2318,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s" s="190">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12">
@@ -2240,18 +2329,18 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C12" t="n" s="192">
-        <v>-2.7392285655624646</v>
+        <v>-3.5233213170882216</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="186">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B13" t="n" s="191">
-        <v>-2.7392285655624646</v>
-      </c>
-      <c r="C13" t="e" s="192">
-        <v>#DIV/0!</v>
+        <v>-3.5233213170882216</v>
+      </c>
+      <c r="C13" t="n" s="192">
+        <v>1.3421772799999999E8</v>
       </c>
     </row>
     <row r="14">
@@ -2275,7 +2364,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="s" s="210">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18">
@@ -2286,15 +2375,15 @@
         <v>0.0</v>
       </c>
       <c r="C18" t="n" s="212">
-        <v>0.028950391649376517</v>
+        <v>0.024376891685690794</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="206">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B19" t="n" s="211">
-        <v>0.028950391649376517</v>
+        <v>0.024376891685690794</v>
       </c>
       <c r="C19" t="n" s="212">
         <v>0.0</v>
@@ -2332,19 +2421,19 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="226">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B24" t="n" s="231">
-        <v>-0.9361906530091433</v>
+        <v>-0.9856008638855045</v>
       </c>
       <c r="C24" t="n" s="232">
-        <v>-0.7192730061032833</v>
+        <v>-0.8696565534786727</v>
       </c>
       <c r="D24" t="n" s="233">
-        <v>-0.10559007281613077</v>
+        <v>-0.1974549415680596</v>
       </c>
       <c r="E24" t="n" s="234">
-        <v>0.028950391649376517</v>
+        <v>0.024376891685690794</v>
       </c>
     </row>
     <row r="25">
@@ -2359,7 +2448,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="238">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28">
@@ -2367,354 +2456,252 @@
         <v>3</v>
       </c>
       <c r="B28" t="s" s="252">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n" s="253">
-        <v>0.20294165134752107</v>
+        <v>0.38055555555555465</v>
       </c>
       <c r="B29" t="n" s="254">
-        <v>0.0</v>
+        <v>4.333333333333333</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n" s="253">
-        <v>0.4869812923614263</v>
+        <v>0.5333333333333332</v>
       </c>
       <c r="B30" t="n" s="254">
-        <v>0.0</v>
+        <v>3.8333333333333335</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n" s="253">
-        <v>-0.6186796122716838</v>
+        <v>0.4222222222222225</v>
       </c>
       <c r="B31" t="n" s="254">
-        <v>0.0</v>
+        <v>5.666666666666667</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n" s="253">
-        <v>0.8467030425455797</v>
+        <v>0.625</v>
       </c>
       <c r="B32" t="n" s="254">
-        <v>0.0</v>
+        <v>3.6666666666666665</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n" s="253">
-        <v>0.6508838283323254</v>
+        <v>0.45555555555555394</v>
       </c>
       <c r="B33" t="n" s="254">
-        <v>0.0</v>
+        <v>3.8333333333333335</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n" s="253">
-        <v>1.1609824497150842</v>
+        <v>0.6083333333333343</v>
       </c>
       <c r="B34" t="n" s="254">
-        <v>0.0</v>
+        <v>2.6666666666666665</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n" s="253">
-        <v>0.7959539365349559</v>
-      </c>
-      <c r="B35" t="n" s="254">
-        <v>0.0</v>
+      <c r="A35" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n" s="253">
-        <v>0.4709151680001552</v>
-      </c>
-      <c r="B36" t="n" s="254">
-        <v>0.0</v>
+      <c r="A36" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n" s="253">
-        <v>-1.0565752195589666</v>
-      </c>
-      <c r="B37" t="n" s="254">
-        <v>2.0</v>
+      <c r="A37" t="s" s="258">
+        <v>42</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
-        <v>1</v>
+      <c r="A38" t="s" s="272">
+        <v>15</v>
+      </c>
+      <c r="B38" t="s" s="272">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s" s="272">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s" s="272">
+        <v>18</v>
+      </c>
+      <c r="E38" t="s" s="272">
+        <v>19</v>
+      </c>
+      <c r="F38" t="s" s="272">
+        <v>20</v>
+      </c>
+      <c r="G38" t="s" s="272">
+        <v>3</v>
+      </c>
+      <c r="H38" t="s" s="272">
+        <v>39</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s">
-        <v>1</v>
+      <c r="A39" t="n" s="273">
+        <v>10181.0</v>
+      </c>
+      <c r="B39" t="n" s="274">
+        <v>1.0276866E7</v>
+      </c>
+      <c r="C39" t="s" s="275">
+        <v>43</v>
+      </c>
+      <c r="D39" t="s" s="276">
+        <v>44</v>
+      </c>
+      <c r="E39" t="s" s="277">
+        <v>50</v>
+      </c>
+      <c r="F39" t="s" s="278">
+        <v>51</v>
+      </c>
+      <c r="G39" t="n" s="279">
+        <v>0.38055555555555465</v>
+      </c>
+      <c r="H39" t="n" s="280">
+        <v>4.333333333333333</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s" s="258">
-        <v>39</v>
+      <c r="A40" t="n" s="273">
+        <v>10188.0</v>
+      </c>
+      <c r="B40" t="n" s="274">
+        <v>1.0276995E7</v>
+      </c>
+      <c r="C40" t="s" s="275">
+        <v>43</v>
+      </c>
+      <c r="D40" t="s" s="276">
+        <v>45</v>
+      </c>
+      <c r="E40" t="s" s="277">
+        <v>50</v>
+      </c>
+      <c r="F40" t="s" s="278">
+        <v>51</v>
+      </c>
+      <c r="G40" t="n" s="279">
+        <v>0.5333333333333332</v>
+      </c>
+      <c r="H40" t="n" s="280">
+        <v>3.8333333333333335</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s" s="272">
-        <v>15</v>
-      </c>
-      <c r="B41" t="s" s="272">
-        <v>16</v>
-      </c>
-      <c r="C41" t="s" s="272">
-        <v>17</v>
-      </c>
-      <c r="D41" t="s" s="272">
-        <v>18</v>
-      </c>
-      <c r="E41" t="s" s="272">
-        <v>19</v>
-      </c>
-      <c r="F41" t="s" s="272">
-        <v>20</v>
-      </c>
-      <c r="G41" t="s" s="272">
-        <v>3</v>
-      </c>
-      <c r="H41" t="s" s="272">
-        <v>36</v>
+      <c r="A41" t="n" s="273">
+        <v>10191.0</v>
+      </c>
+      <c r="B41" t="n" s="274">
+        <v>1.0276981E7</v>
+      </c>
+      <c r="C41" t="s" s="275">
+        <v>43</v>
+      </c>
+      <c r="D41" t="s" s="276">
+        <v>46</v>
+      </c>
+      <c r="E41" t="s" s="277">
+        <v>50</v>
+      </c>
+      <c r="F41" t="s" s="278">
+        <v>51</v>
+      </c>
+      <c r="G41" t="n" s="279">
+        <v>0.4222222222222225</v>
+      </c>
+      <c r="H41" t="n" s="280">
+        <v>5.666666666666667</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n" s="273">
-        <v>10187.0</v>
+        <v>10219.0</v>
       </c>
       <c r="B42" t="n" s="274">
-        <v>9790781.0</v>
+        <v>1.0276831E7</v>
       </c>
       <c r="C42" t="s" s="275">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D42" t="s" s="276">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E42" t="s" s="277">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F42" t="s" s="278">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="G42" t="n" s="279">
-        <v>0.20294165134752107</v>
+        <v>0.625</v>
       </c>
       <c r="H42" t="n" s="280">
-        <v>0.0</v>
+        <v>3.6666666666666665</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n" s="273">
-        <v>10202.0</v>
+        <v>10226.0</v>
       </c>
       <c r="B43" t="n" s="274">
-        <v>1.0277036E7</v>
+        <v>1.0310342E7</v>
       </c>
       <c r="C43" t="s" s="275">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D43" t="s" s="276">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E43" t="s" s="277">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F43" t="s" s="278">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="G43" t="n" s="279">
-        <v>0.4869812923614263</v>
+        <v>0.45555555555555394</v>
       </c>
       <c r="H43" t="n" s="280">
-        <v>0.0</v>
+        <v>3.8333333333333335</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n" s="273">
-        <v>10203.0</v>
+        <v>10230.0</v>
       </c>
       <c r="B44" t="n" s="274">
-        <v>9921470.0</v>
+        <v>1.0351992E7</v>
       </c>
       <c r="C44" t="s" s="275">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D44" t="s" s="276">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E44" t="s" s="277">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F44" t="s" s="278">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="G44" t="n" s="279">
-        <v>-0.6186796122716838</v>
+        <v>0.6083333333333343</v>
       </c>
       <c r="H44" t="n" s="280">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n" s="273">
-        <v>10210.0</v>
-      </c>
-      <c r="B45" t="n" s="274">
-        <v>1.0277015E7</v>
-      </c>
-      <c r="C45" t="s" s="275">
-        <v>21</v>
-      </c>
-      <c r="D45" t="s" s="276">
-        <v>22</v>
-      </c>
-      <c r="E45" t="s" s="277">
-        <v>44</v>
-      </c>
-      <c r="F45" t="s" s="278">
-        <v>34</v>
-      </c>
-      <c r="G45" t="n" s="279">
-        <v>0.8467030425455797</v>
-      </c>
-      <c r="H45" t="n" s="280">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n" s="273">
-        <v>10220.0</v>
-      </c>
-      <c r="B46" t="n" s="274">
-        <v>9760151.0</v>
-      </c>
-      <c r="C46" t="s" s="275">
-        <v>21</v>
-      </c>
-      <c r="D46" t="s" s="276">
-        <v>42</v>
-      </c>
-      <c r="E46" t="s" s="277">
-        <v>44</v>
-      </c>
-      <c r="F46" t="s" s="278">
-        <v>34</v>
-      </c>
-      <c r="G46" t="n" s="279">
-        <v>0.6508838283323254</v>
-      </c>
-      <c r="H46" t="n" s="280">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n" s="273">
-        <v>10224.0</v>
-      </c>
-      <c r="B47" t="n" s="274">
-        <v>9368772.0</v>
-      </c>
-      <c r="C47" t="s" s="275">
-        <v>21</v>
-      </c>
-      <c r="D47" t="s" s="276">
-        <v>23</v>
-      </c>
-      <c r="E47" t="s" s="277">
-        <v>44</v>
-      </c>
-      <c r="F47" t="s" s="278">
-        <v>34</v>
-      </c>
-      <c r="G47" t="n" s="279">
-        <v>1.1609824497150842</v>
-      </c>
-      <c r="H47" t="n" s="280">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n" s="273">
-        <v>10227.0</v>
-      </c>
-      <c r="B48" t="n" s="274">
-        <v>9274382.0</v>
-      </c>
-      <c r="C48" t="s" s="275">
-        <v>21</v>
-      </c>
-      <c r="D48" t="s" s="276">
-        <v>25</v>
-      </c>
-      <c r="E48" t="s" s="277">
-        <v>44</v>
-      </c>
-      <c r="F48" t="s" s="278">
-        <v>34</v>
-      </c>
-      <c r="G48" t="n" s="279">
-        <v>0.7959539365349559</v>
-      </c>
-      <c r="H48" t="n" s="280">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n" s="273">
-        <v>10233.0</v>
-      </c>
-      <c r="B49" t="n" s="274">
-        <v>9805320.0</v>
-      </c>
-      <c r="C49" t="s" s="275">
-        <v>21</v>
-      </c>
-      <c r="D49" t="s" s="276">
-        <v>29</v>
-      </c>
-      <c r="E49" t="s" s="277">
-        <v>44</v>
-      </c>
-      <c r="F49" t="s" s="278">
-        <v>34</v>
-      </c>
-      <c r="G49" t="n" s="279">
-        <v>0.4709151680001552</v>
-      </c>
-      <c r="H49" t="n" s="280">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n" s="273">
-        <v>10238.0</v>
-      </c>
-      <c r="B50" t="n" s="274">
-        <v>1.0276953E7</v>
-      </c>
-      <c r="C50" t="s" s="275">
-        <v>21</v>
-      </c>
-      <c r="D50" t="s" s="276">
-        <v>43</v>
-      </c>
-      <c r="E50" t="s" s="277">
-        <v>44</v>
-      </c>
-      <c r="F50" t="s" s="278">
-        <v>34</v>
-      </c>
-      <c r="G50" t="n" s="279">
-        <v>-1.0565752195589666</v>
-      </c>
-      <c r="H50" t="n" s="280">
-        <v>2.0</v>
+        <v>2.6666666666666665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>